<commit_message>
Files updates (april to may release for Albann)
</commit_message>
<xml_diff>
--- a/gazetteer/gazetteer.xlsx
+++ b/gazetteer/gazetteer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergey.pomerancev\Dropbox\Приложения\Obsidian\git projects\wutc-rus-main\gazetteer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergeypomerantsev/git projects/wutc-rus/gazetteer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D60C00E-EBED-48D9-9ECD-0D9FAFE35148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40F1693-002A-AF43-8311-742AB708B1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{C90B8C3A-B067-4958-B5AD-9BC0D983924F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15520" xr2:uid="{C90B8C3A-B067-4958-B5AD-9BC0D983924F}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="394">
   <si>
     <t>Faroe</t>
   </si>
@@ -1209,6 +1209,18 @@
   </si>
   <si>
     <t>Oswiu</t>
+  </si>
+  <si>
+    <t>Mongfind</t>
+  </si>
+  <si>
+    <t>Монгфинд</t>
+  </si>
+  <si>
+    <t>Flett</t>
+  </si>
+  <si>
+    <t>Флетт</t>
   </si>
 </sst>
 </file>
@@ -1296,7 +1308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1309,7 +1321,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1638,32 +1649,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BEF1417-2C80-4532-AC37-5019930D6A75}">
   <dimension ref="A1:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q45" sqref="Q45"/>
+    <sheetView tabSelected="1" topLeftCell="H40" zoomScale="125" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P53" sqref="P53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.28515625" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="1.7109375" customWidth="1"/>
-    <col min="12" max="12" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.85546875" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.33203125" customWidth="1"/>
+    <col min="9" max="9" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="1.6640625" customWidth="1"/>
+    <col min="12" max="12" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.83203125" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>34</v>
       </c>
@@ -1695,7 +1706,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
@@ -1727,7 +1738,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1762,7 +1773,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -1794,7 +1805,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -1826,7 +1837,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1858,7 +1869,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
@@ -1890,7 +1901,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
@@ -1925,7 +1936,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1957,7 +1968,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>0</v>
       </c>
@@ -1992,7 +2003,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -2018,7 +2029,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>1</v>
       </c>
@@ -2044,7 +2055,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
@@ -2070,7 +2081,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
@@ -2096,7 +2107,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
@@ -2122,7 +2133,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
@@ -2148,7 +2159,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>12</v>
       </c>
@@ -2174,7 +2185,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>26</v>
       </c>
@@ -2194,7 +2205,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>25</v>
       </c>
@@ -2220,7 +2231,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
@@ -2246,7 +2257,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
@@ -2272,7 +2283,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>16</v>
       </c>
@@ -2298,7 +2309,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>18</v>
       </c>
@@ -2324,7 +2335,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>27</v>
       </c>
@@ -2350,7 +2361,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>7</v>
       </c>
@@ -2376,7 +2387,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>3</v>
       </c>
@@ -2396,7 +2407,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>9</v>
       </c>
@@ -2422,7 +2433,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>23</v>
       </c>
@@ -2442,7 +2453,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>5</v>
       </c>
@@ -2468,7 +2479,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>4</v>
       </c>
@@ -2494,7 +2505,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>59</v>
       </c>
@@ -2520,7 +2531,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I32" t="s">
         <v>321</v>
       </c>
@@ -2540,7 +2551,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="33" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="9:16" x14ac:dyDescent="0.2">
       <c r="I33" t="s">
         <v>326</v>
       </c>
@@ -2560,7 +2571,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="34" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="9:16" x14ac:dyDescent="0.2">
       <c r="I34" t="s">
         <v>331</v>
       </c>
@@ -2580,7 +2591,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="35" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="9:16" x14ac:dyDescent="0.2">
       <c r="I35" t="s">
         <v>333</v>
       </c>
@@ -2600,7 +2611,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="36" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="9:16" x14ac:dyDescent="0.2">
       <c r="I36" t="s">
         <v>335</v>
       </c>
@@ -2620,7 +2631,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="37" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="9:16" x14ac:dyDescent="0.2">
       <c r="I37" t="s">
         <v>336</v>
       </c>
@@ -2640,7 +2651,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="38" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="9:16" x14ac:dyDescent="0.2">
       <c r="I38" t="s">
         <v>342</v>
       </c>
@@ -2660,7 +2671,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="39" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="9:16" x14ac:dyDescent="0.2">
       <c r="I39" t="s">
         <v>344</v>
       </c>
@@ -2680,7 +2691,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="40" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="9:16" x14ac:dyDescent="0.2">
       <c r="I40" t="s">
         <v>350</v>
       </c>
@@ -2700,7 +2711,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="41" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="9:16" x14ac:dyDescent="0.2">
       <c r="I41" t="s">
         <v>354</v>
       </c>
@@ -2720,7 +2731,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="42" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="9:16" x14ac:dyDescent="0.2">
       <c r="I42" t="s">
         <v>387</v>
       </c>
@@ -2740,7 +2751,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="43" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="9:16" x14ac:dyDescent="0.2">
       <c r="L43" t="s">
         <v>266</v>
       </c>
@@ -2754,7 +2765,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="44" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="9:16" x14ac:dyDescent="0.2">
       <c r="L44" t="s">
         <v>292</v>
       </c>
@@ -2768,7 +2779,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="45" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="9:16" x14ac:dyDescent="0.2">
       <c r="L45" t="s">
         <v>294</v>
       </c>
@@ -2778,9 +2789,9 @@
       <c r="O45" s="9" t="s">
         <v>389</v>
       </c>
-      <c r="P45" s="11"/>
-    </row>
-    <row r="46" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="P45" s="10"/>
+    </row>
+    <row r="46" spans="9:16" x14ac:dyDescent="0.2">
       <c r="L46" t="s">
         <v>295</v>
       </c>
@@ -2794,7 +2805,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="47" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="9:16" x14ac:dyDescent="0.2">
       <c r="L47" t="s">
         <v>296</v>
       </c>
@@ -2808,7 +2819,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="48" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="9:16" x14ac:dyDescent="0.2">
       <c r="L48" t="s">
         <v>301</v>
       </c>
@@ -2822,7 +2833,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="49" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="12:16" x14ac:dyDescent="0.2">
       <c r="L49" t="s">
         <v>306</v>
       </c>
@@ -2836,7 +2847,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="50" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="12:16" x14ac:dyDescent="0.2">
       <c r="L50" t="s">
         <v>308</v>
       </c>
@@ -2846,11 +2857,11 @@
       <c r="O50" t="s">
         <v>338</v>
       </c>
-      <c r="P50" s="10" t="s">
+      <c r="P50" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="51" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="12:16" x14ac:dyDescent="0.2">
       <c r="L51" t="s">
         <v>311</v>
       </c>
@@ -2864,7 +2875,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="52" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="12:16" x14ac:dyDescent="0.2">
       <c r="L52" t="s">
         <v>346</v>
       </c>
@@ -2878,7 +2889,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="53" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="12:16" x14ac:dyDescent="0.2">
       <c r="L53" t="s">
         <v>347</v>
       </c>
@@ -2892,7 +2903,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="54" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="12:16" x14ac:dyDescent="0.2">
       <c r="L54" t="s">
         <v>360</v>
       </c>
@@ -2906,7 +2917,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="55" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="12:16" x14ac:dyDescent="0.2">
       <c r="L55" t="s">
         <v>362</v>
       </c>
@@ -2920,71 +2931,83 @@
         <v>369</v>
       </c>
     </row>
-    <row r="56" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="12:16" x14ac:dyDescent="0.2">
       <c r="L56" t="s">
         <v>364</v>
       </c>
       <c r="M56" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="57" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="O56" t="s">
+        <v>390</v>
+      </c>
+      <c r="P56" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="57" spans="12:16" x14ac:dyDescent="0.2">
       <c r="L57" t="s">
         <v>366</v>
       </c>
       <c r="M57" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="58" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="O57" t="s">
+        <v>392</v>
+      </c>
+      <c r="P57" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="58" spans="12:16" x14ac:dyDescent="0.2">
       <c r="L58" t="s">
         <v>370</v>
       </c>
-      <c r="M58" s="10" t="s">
+      <c r="M58" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="59" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="12:16" x14ac:dyDescent="0.2">
       <c r="L59" t="s">
         <v>371</v>
       </c>
-      <c r="M59" s="10" t="s">
+      <c r="M59" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="60" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="12:16" x14ac:dyDescent="0.2">
       <c r="L60" t="s">
         <v>372</v>
       </c>
-      <c r="M60" s="10" t="s">
+      <c r="M60" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="61" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="12:16" x14ac:dyDescent="0.2">
       <c r="L61" t="s">
         <v>373</v>
       </c>
-      <c r="M61" s="10" t="s">
+      <c r="M61" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="62" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="12:16" x14ac:dyDescent="0.2">
       <c r="L62" t="s">
         <v>374</v>
       </c>
-      <c r="M62" s="10" t="s">
+      <c r="M62" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="63" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="12:16" x14ac:dyDescent="0.2">
       <c r="L63" t="s">
         <v>375</v>
       </c>
-      <c r="M63" s="10" t="s">
+      <c r="M63" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="64" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="12:16" x14ac:dyDescent="0.2">
       <c r="L64" t="s">
         <v>382</v>
       </c>
@@ -2992,7 +3015,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="65" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L65" t="s">
         <v>384</v>
       </c>

</xml_diff>